<commit_message>
Finished first draft, converted to function
</commit_message>
<xml_diff>
--- a/APCE_data_8_12_2020.xlsx
+++ b/APCE_data_8_12_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\R\Whelan_Lab_Binding_Fit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C6BD26-D766-4476-8BDB-122CC3883891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3D1174-30E6-468F-A6F5-88882B0B79A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{34433921-8FF8-4ADD-82E8-AFC60609B7F1}"/>
+    <workbookView xWindow="14604" yWindow="4584" windowWidth="23304" windowHeight="11544" activeTab="2" xr2:uid="{34433921-8FF8-4ADD-82E8-AFC60609B7F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Prep" sheetId="1" r:id="rId1"/>
@@ -3185,7 +3185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9711ADB-96EB-4071-8929-49EE340410FF}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="71" workbookViewId="0">
+    <sheetView zoomScale="71" workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -4048,8 +4048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4C7CCB-5423-49C1-9CF7-B848D7E1AB34}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5283,8 +5283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB74E3DA-CFB1-4661-A391-D3A69588A4A2}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>